<commit_message>
Added the characterization factors of plastic resin from the MariLCA group + correct a mistake that was dividing the S matrix for non-plastic flows by 1,000,000.
</commit_message>
<xml_diff>
--- a/Data/Environmental_data/plastic_resin_compositions.xlsx
+++ b/Data/Environmental_data/plastic_resin_compositions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\OpenIOCanada\Data\Environmental_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F421A2C-6118-4E03-92D4-A8ECF93296DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593947F-89B2-424E-A7CE-2B590E498AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="G2" s="2">
         <v>0.09</v>
@@ -540,7 +540,9 @@
       <c r="I2" s="2">
         <v>0.77</v>
       </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2">
+        <v>0.01</v>
+      </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -557,7 +559,9 @@
       <c r="I3" s="2">
         <v>0.05</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2">
+        <v>0.01</v>
+      </c>
       <c r="K3" s="2">
         <v>0.08</v>
       </c>
@@ -574,7 +578,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -601,7 +605,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -630,7 +634,7 @@
         <v>0.3</v>
       </c>
       <c r="E6" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>0.17</v>
       </c>
       <c r="F6" s="2">
         <v>0.25</v>
@@ -721,8 +725,12 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="E10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.02</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2">
         <v>0.05</v>
@@ -747,7 +755,7 @@
         <v>0.1</v>
       </c>
       <c r="E11" s="2">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
       <c r="F11" s="2">
         <v>0.25</v>
@@ -916,7 +924,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="K19" s="2">
         <v>0.08</v>

</xml_diff>